<commit_message>
moved engineer comments to comment section at the bottom
</commit_message>
<xml_diff>
--- a/jobcard_template.xlsx
+++ b/jobcard_template.xlsx
@@ -380,7 +380,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -505,8 +505,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -515,6 +515,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -728,12 +732,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B2:Z37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA10" activeCellId="0" sqref="AA10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -754,7 +758,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="3.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="1.71"/>
   </cols>
   <sheetData>
@@ -1534,16 +1538,16 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
       <c r="L31" s="32"/>
       <c r="M31" s="32"/>
       <c r="N31" s="32"/>
@@ -1563,16 +1567,16 @@
       <c r="Z31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
       <c r="L32" s="32"/>
       <c r="M32" s="32"/>
       <c r="N32" s="32"/>
@@ -1592,16 +1596,16 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
       <c r="L33" s="32" t="s">
         <v>49</v>
       </c>
@@ -1616,23 +1620,23 @@
       <c r="S33" s="33"/>
       <c r="T33" s="8"/>
       <c r="U33" s="8"/>
-      <c r="V33" s="34"/>
-      <c r="W33" s="34"/>
-      <c r="X33" s="34"/>
-      <c r="Y33" s="34"/>
-      <c r="Z33" s="34"/>
+      <c r="V33" s="35"/>
+      <c r="W33" s="35"/>
+      <c r="X33" s="35"/>
+      <c r="Y33" s="35"/>
+      <c r="Z33" s="35"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
       <c r="L34" s="33" t="s">
         <v>51</v>
       </c>
@@ -1648,31 +1652,31 @@
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
-      <c r="Y34" s="35"/>
-      <c r="Z34" s="35"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="36"/>
     </row>
     <row r="35" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="36"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="25"/>
       <c r="E35" s="25"/>
-      <c r="G35" s="37" t="s">
+      <c r="G35" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="38"/>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="38"/>
-      <c r="R35" s="38"/>
-      <c r="S35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39"/>
+      <c r="O35" s="39"/>
+      <c r="P35" s="39"/>
+      <c r="Q35" s="39"/>
+      <c r="R35" s="39"/>
+      <c r="S35" s="39"/>
       <c r="V35" s="4" t="s">
         <v>54</v>
       </c>
@@ -1690,22 +1694,22 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="37" t="s">
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="O36" s="37"/>
-      <c r="P36" s="37"/>
-      <c r="Q36" s="37"/>
-      <c r="R36" s="39"/>
-      <c r="S36" s="39"/>
-      <c r="T36" s="39"/>
-      <c r="U36" s="39"/>
+      <c r="O36" s="38"/>
+      <c r="P36" s="38"/>
+      <c r="Q36" s="38"/>
+      <c r="R36" s="40"/>
+      <c r="S36" s="40"/>
+      <c r="T36" s="40"/>
+      <c r="U36" s="40"/>
       <c r="V36" s="4" t="s">
         <v>57</v>
       </c>
@@ -1746,7 +1750,7 @@
       <c r="Z37" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="177">
+  <mergeCells count="178">
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="V3:Z5"/>
     <mergeCell ref="D6:E6"/>
@@ -1884,12 +1888,13 @@
     <mergeCell ref="T29:U29"/>
     <mergeCell ref="V29:X29"/>
     <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="B30:K34"/>
+    <mergeCell ref="B30:K30"/>
     <mergeCell ref="L30:O30"/>
     <mergeCell ref="P30:S30"/>
     <mergeCell ref="T30:U30"/>
     <mergeCell ref="V30:X30"/>
     <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="B31:K34"/>
     <mergeCell ref="L31:O31"/>
     <mergeCell ref="P31:S31"/>
     <mergeCell ref="T31:U31"/>
@@ -1927,7 +1932,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>